<commit_message>
Removed data from the excel sheet
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caleb Yeboah\PycharmProjects\pythonProject\Projects\WhatsApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F751A39-6434-4738-AB32-2AFA3FD7614A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A24C9A-27C2-42CE-9D4A-23726BAC88E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Settings</t>
   </si>
@@ -40,28 +40,16 @@
     <t>Minutes</t>
   </si>
   <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>+233501380504</t>
-  </si>
-  <si>
-    <t>Hello, Good afternoon</t>
-  </si>
-  <si>
     <t>Values</t>
   </si>
   <si>
     <t>Keys</t>
   </si>
   <si>
-    <t>+233558081606</t>
-  </si>
-  <si>
-    <t>Hi, Good afternoon</t>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>TextMessage</t>
   </si>
 </sst>
 </file>
@@ -121,8 +109,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FD636097-A705-4136-A221-E2B38706C53B}" name="Table1" displayName="Table1" ref="A1:B24" totalsRowShown="0">
   <autoFilter ref="A1:B24" xr:uid="{FD636097-A705-4136-A221-E2B38706C53B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{806EF865-566F-4814-93EE-E65B3417919F}" name="Number"/>
-    <tableColumn id="2" xr3:uid="{2123F6B6-C813-47BE-A972-FE20AB719BCB}" name="Text"/>
+    <tableColumn id="1" xr3:uid="{806EF865-566F-4814-93EE-E65B3417919F}" name="PhoneNumber"/>
+    <tableColumn id="2" xr3:uid="{2123F6B6-C813-47BE-A972-FE20AB719BCB}" name="TextMessage"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -406,7 +394,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -417,27 +405,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
+      <c r="A3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -466,10 +444,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>